<commit_message>
Fix: final composition name in excel
</commit_message>
<xml_diff>
--- a/files/utils/BASE_FRAC_MOLAR_Overall.xlsx
+++ b/files/utils/BASE_FRAC_MOLAR_Overall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\pythonProject\CalculosFrequencia\filtercomp\files\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\pythonProject\filtercomp\files\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4556F49-5370-4A5C-86F0-0B0D45195528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B4D857-2A29-4E1D-8B8E-EAB955404209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20994B5E-CD57-4B76-9F13-AB691988E7F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{20994B5E-CD57-4B76-9F13-AB691988E7F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Composição" sheetId="1" r:id="rId1"/>
@@ -504,9 +504,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -544,7 +544,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -650,7 +650,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -792,7 +792,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -803,7 +803,7 @@
   <dimension ref="A1:IP69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="XEH1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="XEH62" sqref="XEH62"/>
     </sheetView>
   </sheetViews>

</xml_diff>